<commit_message>
finished new image selection process; copied selected images to new folder
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2/trial_list_generator/scenecat_stimulus_selection_summary.xlsx
+++ b/scene_cat_exp_2023.2/trial_list_generator/scenecat_stimulus_selection_summary.xlsx
@@ -418,8 +418,10 @@
       <c r="C2">
         <v>55</v>
       </c>
-      <c r="D2">
-        <v>4</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E2">
         <v>1</v>
@@ -453,8 +455,10 @@
       <c r="C3">
         <v>11.05555555555556</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E3">
         <v>1</v>
@@ -488,8 +492,10 @@
       <c r="C4">
         <v>39.5</v>
       </c>
-      <c r="D4">
-        <v>2</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E4">
         <v>1</v>
@@ -523,8 +529,10 @@
       <c r="C5">
         <v>52.171875</v>
       </c>
-      <c r="D5">
-        <v>4</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E5">
         <v>1</v>
@@ -558,8 +566,10 @@
       <c r="C6">
         <v>76.36904761904762</v>
       </c>
-      <c r="D6">
-        <v>9</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E6">
         <v>1</v>
@@ -593,8 +603,10 @@
       <c r="C7">
         <v>71.17948717948718</v>
       </c>
-      <c r="D7">
-        <v>8</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E7">
         <v>1</v>
@@ -628,8 +640,10 @@
       <c r="C8">
         <v>54.26136363636364</v>
       </c>
-      <c r="D8">
-        <v>5</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E8">
         <v>0</v>
@@ -663,8 +677,10 @@
       <c r="C9">
         <v>81.12162162162161</v>
       </c>
-      <c r="D9">
-        <v>10</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E9">
         <v>1</v>
@@ -698,8 +714,10 @@
       <c r="C10">
         <v>74.22222222222223</v>
       </c>
-      <c r="D10">
-        <v>8</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E10">
         <v>1</v>
@@ -733,8 +751,10 @@
       <c r="C11">
         <v>58.01190476190476</v>
       </c>
-      <c r="D11">
-        <v>5</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E11">
         <v>1</v>
@@ -768,8 +788,10 @@
       <c r="C12">
         <v>65.28378378378379</v>
       </c>
-      <c r="D12">
-        <v>6</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E12">
         <v>1</v>
@@ -803,8 +825,10 @@
       <c r="C13">
         <v>22.42105263157895</v>
       </c>
-      <c r="D13">
-        <v>1</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E13">
         <v>1</v>
@@ -838,8 +862,10 @@
       <c r="C14">
         <v>62.22222222222223</v>
       </c>
-      <c r="D14">
-        <v>6</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E14">
         <v>0</v>
@@ -873,8 +899,10 @@
       <c r="C15">
         <v>53.57954545454545</v>
       </c>
-      <c r="D15">
-        <v>5</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E15">
         <v>0</v>
@@ -908,8 +936,10 @@
       <c r="C16">
         <v>64.29166666666667</v>
       </c>
-      <c r="D16">
-        <v>6</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E16">
         <v>1</v>
@@ -943,8 +973,10 @@
       <c r="C17">
         <v>67.77142857142857</v>
       </c>
-      <c r="D17">
-        <v>7</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E17">
         <v>1</v>
@@ -978,8 +1010,10 @@
       <c r="C18">
         <v>59.05555555555556</v>
       </c>
-      <c r="D18">
-        <v>5</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1013,8 +1047,10 @@
       <c r="C19">
         <v>44.94871794871795</v>
       </c>
-      <c r="D19">
-        <v>3</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1048,8 +1084,10 @@
       <c r="C20">
         <v>69.85526315789474</v>
       </c>
-      <c r="D20">
-        <v>7</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1083,8 +1121,10 @@
       <c r="C21">
         <v>30.45833333333334</v>
       </c>
-      <c r="D21">
-        <v>2</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1118,8 +1158,10 @@
       <c r="C22">
         <v>58.68571428571429</v>
       </c>
-      <c r="D22">
-        <v>5</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1153,8 +1195,10 @@
       <c r="C23">
         <v>58.92424242424242</v>
       </c>
-      <c r="D23">
-        <v>5</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1188,8 +1232,10 @@
       <c r="C24">
         <v>60.09302325581395</v>
       </c>
-      <c r="D24">
-        <v>5</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1223,8 +1269,10 @@
       <c r="C25">
         <v>78.2948717948718</v>
       </c>
-      <c r="D25">
-        <v>9</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1258,8 +1306,10 @@
       <c r="C26">
         <v>50.10714285714286</v>
       </c>
-      <c r="D26">
-        <v>3</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1293,8 +1343,10 @@
       <c r="C27">
         <v>85.08108108108108</v>
       </c>
-      <c r="D27">
-        <v>10</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1328,8 +1380,10 @@
       <c r="C28">
         <v>70.22222222222223</v>
       </c>
-      <c r="D28">
-        <v>7</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1363,8 +1417,10 @@
       <c r="C29">
         <v>75.62162162162161</v>
       </c>
-      <c r="D29">
-        <v>9</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1398,8 +1454,10 @@
       <c r="C30">
         <v>85.68181818181819</v>
       </c>
-      <c r="D30">
-        <v>10</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1433,8 +1491,10 @@
       <c r="C31">
         <v>41.34722222222223</v>
       </c>
-      <c r="D31">
-        <v>2</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1468,8 +1528,10 @@
       <c r="C32">
         <v>55.31081081081081</v>
       </c>
-      <c r="D32">
-        <v>5</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1503,8 +1565,10 @@
       <c r="C33">
         <v>64.09999999999999</v>
       </c>
-      <c r="D33">
-        <v>6</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1538,8 +1602,10 @@
       <c r="C34">
         <v>23.48837209302326</v>
       </c>
-      <c r="D34">
-        <v>1</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1573,8 +1639,10 @@
       <c r="C35">
         <v>60.03571428571429</v>
       </c>
-      <c r="D35">
-        <v>5</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1608,8 +1676,10 @@
       <c r="C36">
         <v>29.63265306122449</v>
       </c>
-      <c r="D36">
-        <v>2</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1643,8 +1713,10 @@
       <c r="C37">
         <v>79.97142857142858</v>
       </c>
-      <c r="D37">
-        <v>9</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1678,8 +1750,10 @@
       <c r="C38">
         <v>56.46774193548387</v>
       </c>
-      <c r="D38">
-        <v>4</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1713,8 +1787,10 @@
       <c r="C39">
         <v>66.625</v>
       </c>
-      <c r="D39">
-        <v>7</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1748,8 +1824,10 @@
       <c r="C40">
         <v>42.63157894736842</v>
       </c>
-      <c r="D40">
-        <v>3</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1783,8 +1861,10 @@
       <c r="C41">
         <v>6.878378378378379</v>
       </c>
-      <c r="D41">
-        <v>1</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1818,8 +1898,10 @@
       <c r="C42">
         <v>58.27659574468085</v>
       </c>
-      <c r="D42">
-        <v>5</v>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1853,8 +1935,10 @@
       <c r="C43">
         <v>56.6969696969697</v>
       </c>
-      <c r="D43">
-        <v>4</v>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1888,8 +1972,10 @@
       <c r="C44">
         <v>56.84722222222222</v>
       </c>
-      <c r="D44">
-        <v>4</v>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1923,8 +2009,10 @@
       <c r="C45">
         <v>58.42391304347826</v>
       </c>
-      <c r="D45">
-        <v>5</v>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1958,8 +2046,10 @@
       <c r="C46">
         <v>75.47674418604652</v>
       </c>
-      <c r="D46">
-        <v>8</v>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1993,8 +2083,10 @@
       <c r="C47">
         <v>50.28409090909091</v>
       </c>
-      <c r="D47">
-        <v>3</v>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E47">
         <v>1</v>
@@ -2028,8 +2120,10 @@
       <c r="C48">
         <v>50.73076923076923</v>
       </c>
-      <c r="D48">
-        <v>4</v>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2063,8 +2157,10 @@
       <c r="C49">
         <v>60.76315789473685</v>
       </c>
-      <c r="D49">
-        <v>5</v>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2098,8 +2194,10 @@
       <c r="C50">
         <v>80.85869565217391</v>
       </c>
-      <c r="D50">
-        <v>10</v>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2133,8 +2231,10 @@
       <c r="C51">
         <v>71.1125</v>
       </c>
-      <c r="D51">
-        <v>8</v>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E51">
         <v>1</v>
@@ -2168,8 +2268,10 @@
       <c r="C52">
         <v>55.025</v>
       </c>
-      <c r="D52">
-        <v>4</v>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2203,8 +2305,10 @@
       <c r="C53">
         <v>65.43421052631579</v>
       </c>
-      <c r="D53">
-        <v>6</v>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2238,8 +2342,10 @@
       <c r="C54">
         <v>69.44444444444444</v>
       </c>
-      <c r="D54">
-        <v>8</v>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2273,8 +2379,10 @@
       <c r="C55">
         <v>52.42424242424242</v>
       </c>
-      <c r="D55">
-        <v>3</v>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2308,8 +2416,10 @@
       <c r="C56">
         <v>62.52777777777777</v>
       </c>
-      <c r="D56">
-        <v>6</v>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2343,8 +2453,10 @@
       <c r="C57">
         <v>74.79729729729729</v>
       </c>
-      <c r="D57">
-        <v>9</v>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2378,8 +2490,10 @@
       <c r="C58">
         <v>56.93939393939394</v>
       </c>
-      <c r="D58">
-        <v>4</v>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2413,8 +2527,10 @@
       <c r="C59">
         <v>58.48529411764706</v>
       </c>
-      <c r="D59">
-        <v>5</v>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2448,8 +2564,10 @@
       <c r="C60">
         <v>52.93181818181819</v>
       </c>
-      <c r="D60">
-        <v>5</v>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E60">
         <v>0</v>
@@ -2483,8 +2601,10 @@
       <c r="C61">
         <v>64.65789473684211</v>
       </c>
-      <c r="D61">
-        <v>6</v>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E61">
         <v>0</v>
@@ -2518,8 +2638,10 @@
       <c r="C62">
         <v>54.44</v>
       </c>
-      <c r="D62">
-        <v>4</v>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2553,8 +2675,10 @@
       <c r="C63">
         <v>71.390625</v>
       </c>
-      <c r="D63">
-        <v>8</v>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2588,8 +2712,10 @@
       <c r="C64">
         <v>82.27272727272728</v>
       </c>
-      <c r="D64">
-        <v>10</v>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2623,8 +2749,10 @@
       <c r="C65">
         <v>59.83333333333334</v>
       </c>
-      <c r="D65">
-        <v>5</v>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2658,8 +2786,10 @@
       <c r="C66">
         <v>43.83870967741936</v>
       </c>
-      <c r="D66">
-        <v>2</v>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2693,8 +2823,10 @@
       <c r="C67">
         <v>59.91891891891892</v>
       </c>
-      <c r="D67">
-        <v>5</v>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2728,8 +2860,10 @@
       <c r="C68">
         <v>9.382352941176471</v>
       </c>
-      <c r="D68">
-        <v>1</v>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2763,8 +2897,10 @@
       <c r="C69">
         <v>48.02941176470588</v>
       </c>
-      <c r="D69">
-        <v>3</v>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2798,8 +2934,10 @@
       <c r="C70">
         <v>68.14516129032258</v>
       </c>
-      <c r="D70">
-        <v>7</v>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2833,8 +2971,10 @@
       <c r="C71">
         <v>65.97872340425532</v>
       </c>
-      <c r="D71">
-        <v>6</v>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2868,8 +3008,10 @@
       <c r="C72">
         <v>72.515625</v>
       </c>
-      <c r="D72">
-        <v>9</v>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2903,8 +3045,10 @@
       <c r="C73">
         <v>66.51515151515152</v>
       </c>
-      <c r="D73">
-        <v>7</v>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E73">
         <v>1</v>
@@ -2938,8 +3082,10 @@
       <c r="C74">
         <v>34.28787878787879</v>
       </c>
-      <c r="D74">
-        <v>1</v>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E74">
         <v>1</v>
@@ -2973,8 +3119,10 @@
       <c r="C75">
         <v>40.01428571428572</v>
       </c>
-      <c r="D75">
-        <v>2</v>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3008,8 +3156,10 @@
       <c r="C76">
         <v>64.81944444444444</v>
       </c>
-      <c r="D76">
-        <v>6</v>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3043,8 +3193,10 @@
       <c r="C77">
         <v>77.24242424242425</v>
       </c>
-      <c r="D77">
-        <v>10</v>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E77">
         <v>1</v>
@@ -3078,8 +3230,10 @@
       <c r="C78">
         <v>60.74242424242424</v>
       </c>
-      <c r="D78">
-        <v>5</v>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E78">
         <v>1</v>
@@ -3113,8 +3267,10 @@
       <c r="C79">
         <v>60</v>
       </c>
-      <c r="D79">
-        <v>5</v>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E79">
         <v>0</v>
@@ -3148,8 +3304,10 @@
       <c r="C80">
         <v>65.81944444444444</v>
       </c>
-      <c r="D80">
-        <v>7</v>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E80">
         <v>1</v>
@@ -3183,8 +3341,10 @@
       <c r="C81">
         <v>61.54545454545455</v>
       </c>
-      <c r="D81">
-        <v>6</v>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E81">
         <v>0</v>
@@ -3218,8 +3378,10 @@
       <c r="C82">
         <v>52.59259259259259</v>
       </c>
-      <c r="D82">
-        <v>3</v>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E82">
         <v>1</v>
@@ -3253,8 +3415,10 @@
       <c r="C83">
         <v>61.76136363636364</v>
       </c>
-      <c r="D83">
-        <v>6</v>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E83">
         <v>0</v>
@@ -3288,8 +3452,10 @@
       <c r="C84">
         <v>58.18421052631579</v>
       </c>
-      <c r="D84">
-        <v>5</v>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E84">
         <v>0</v>
@@ -3323,8 +3489,10 @@
       <c r="C85">
         <v>45.26470588235294</v>
       </c>
-      <c r="D85">
-        <v>2</v>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E85">
         <v>1</v>
@@ -3358,8 +3526,10 @@
       <c r="C86">
         <v>53.59090909090909</v>
       </c>
-      <c r="D86">
-        <v>4</v>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E86">
         <v>1</v>
@@ -3393,8 +3563,10 @@
       <c r="C87">
         <v>76.25925925925925</v>
       </c>
-      <c r="D87">
-        <v>10</v>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E87">
         <v>1</v>
@@ -3428,8 +3600,10 @@
       <c r="C88">
         <v>6.96875</v>
       </c>
-      <c r="D88">
-        <v>1</v>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E88">
         <v>1</v>
@@ -3463,8 +3637,10 @@
       <c r="C89">
         <v>69.09722222222223</v>
       </c>
-      <c r="D89">
-        <v>8</v>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E89">
         <v>1</v>
@@ -3498,8 +3674,10 @@
       <c r="C90">
         <v>39.98484848484848</v>
       </c>
-      <c r="D90">
-        <v>2</v>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E90">
         <v>1</v>
@@ -3533,8 +3711,10 @@
       <c r="C91">
         <v>61.12121212121212</v>
       </c>
-      <c r="D91">
-        <v>5</v>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E91">
         <v>1</v>
@@ -3568,8 +3748,10 @@
       <c r="C92">
         <v>62.13414634146342</v>
       </c>
-      <c r="D92">
-        <v>6</v>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E92">
         <v>0</v>
@@ -3603,8 +3785,10 @@
       <c r="C93">
         <v>58.21951219512195</v>
       </c>
-      <c r="D93">
-        <v>5</v>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E93">
         <v>0</v>
@@ -3638,8 +3822,10 @@
       <c r="C94">
         <v>82.68571428571428</v>
       </c>
-      <c r="D94">
-        <v>10</v>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E94">
         <v>1</v>
@@ -3673,8 +3859,10 @@
       <c r="C95">
         <v>47.84375</v>
       </c>
-      <c r="D95">
-        <v>3</v>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E95">
         <v>1</v>
@@ -3708,8 +3896,10 @@
       <c r="C96">
         <v>68.21875</v>
       </c>
-      <c r="D96">
-        <v>7</v>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E96">
         <v>1</v>
@@ -3743,8 +3933,10 @@
       <c r="C97">
         <v>57.01428571428572</v>
       </c>
-      <c r="D97">
-        <v>4</v>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E97">
         <v>1</v>
@@ -3778,8 +3970,10 @@
       <c r="C98">
         <v>62.22058823529412</v>
       </c>
-      <c r="D98">
-        <v>6</v>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E98">
         <v>1</v>
@@ -3813,8 +4007,10 @@
       <c r="C99">
         <v>74.94117647058823</v>
       </c>
-      <c r="D99">
-        <v>9</v>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E99">
         <v>1</v>
@@ -3848,8 +4044,10 @@
       <c r="C100">
         <v>36.41379310344828</v>
       </c>
-      <c r="D100">
-        <v>1</v>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E100">
         <v>1</v>
@@ -3883,8 +4081,10 @@
       <c r="C101">
         <v>64.96969696969697</v>
       </c>
-      <c r="D101">
-        <v>6</v>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E101">
         <v>1</v>
@@ -3918,8 +4118,10 @@
       <c r="C102">
         <v>59.63414634146342</v>
       </c>
-      <c r="D102">
-        <v>5</v>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E102">
         <v>0</v>
@@ -3953,8 +4155,10 @@
       <c r="C103">
         <v>71.421875</v>
       </c>
-      <c r="D103">
-        <v>8</v>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E103">
         <v>1</v>
@@ -3988,8 +4192,10 @@
       <c r="C104">
         <v>72.11666666666667</v>
       </c>
-      <c r="D104">
-        <v>9</v>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E104">
         <v>1</v>
@@ -4023,8 +4229,10 @@
       <c r="C105">
         <v>58.32142857142857</v>
       </c>
-      <c r="D105">
-        <v>5</v>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E105">
         <v>1</v>
@@ -4058,8 +4266,10 @@
       <c r="C106">
         <v>50.62790697674419</v>
       </c>
-      <c r="D106">
-        <v>4</v>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E106">
         <v>1</v>
@@ -4093,8 +4303,10 @@
       <c r="C107">
         <v>79.70238095238095</v>
       </c>
-      <c r="D107">
-        <v>9</v>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E107">
         <v>1</v>
@@ -4128,8 +4340,10 @@
       <c r="C108">
         <v>31.98936170212766</v>
       </c>
-      <c r="D108">
-        <v>3</v>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E108">
         <v>1</v>
@@ -4163,8 +4377,10 @@
       <c r="C109">
         <v>20.73170731707317</v>
       </c>
-      <c r="D109">
-        <v>2</v>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E109">
         <v>1</v>
@@ -4198,8 +4414,10 @@
       <c r="C110">
         <v>54.9390243902439</v>
       </c>
-      <c r="D110">
-        <v>4</v>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E110">
         <v>0</v>
@@ -4233,8 +4451,10 @@
       <c r="C111">
         <v>31.22340425531915</v>
       </c>
-      <c r="D111">
-        <v>2</v>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E111">
         <v>1</v>
@@ -4268,8 +4488,10 @@
       <c r="C112">
         <v>54.5</v>
       </c>
-      <c r="D112">
-        <v>4</v>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E112">
         <v>0</v>
@@ -4303,8 +4525,10 @@
       <c r="C113">
         <v>80.05000000000001</v>
       </c>
-      <c r="D113">
-        <v>10</v>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E113">
         <v>1</v>
@@ -4338,8 +4562,10 @@
       <c r="C114">
         <v>43.6025641025641</v>
       </c>
-      <c r="D114">
-        <v>3</v>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E114">
         <v>1</v>
@@ -4373,8 +4599,10 @@
       <c r="C115">
         <v>76.68604651162791</v>
       </c>
-      <c r="D115">
-        <v>9</v>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E115">
         <v>1</v>
@@ -4408,8 +4636,10 @@
       <c r="C116">
         <v>51.13953488372093</v>
       </c>
-      <c r="D116">
-        <v>5</v>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E116">
         <v>1</v>
@@ -4443,8 +4673,10 @@
       <c r="C117">
         <v>11.125</v>
       </c>
-      <c r="D117">
-        <v>1</v>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E117">
         <v>1</v>
@@ -4478,8 +4710,10 @@
       <c r="C118">
         <v>76.63414634146342</v>
       </c>
-      <c r="D118">
-        <v>8</v>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E118">
         <v>1</v>
@@ -4513,8 +4747,10 @@
       <c r="C119">
         <v>60.95454545454545</v>
       </c>
-      <c r="D119">
-        <v>5</v>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E119">
         <v>1</v>
@@ -4548,8 +4784,10 @@
       <c r="C120">
         <v>88.69565217391303</v>
       </c>
-      <c r="D120">
-        <v>10</v>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E120">
         <v>1</v>
@@ -4583,8 +4821,10 @@
       <c r="C121">
         <v>54.64705882352941</v>
       </c>
-      <c r="D121">
-        <v>4</v>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E121">
         <v>0</v>
@@ -4618,8 +4858,10 @@
       <c r="C122">
         <v>71.96590909090909</v>
       </c>
-      <c r="D122">
-        <v>7</v>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E122">
         <v>1</v>
@@ -4653,8 +4895,10 @@
       <c r="C123">
         <v>54.74242424242424</v>
       </c>
-      <c r="D123">
-        <v>4</v>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E123">
         <v>0</v>
@@ -4688,8 +4932,10 @@
       <c r="C124">
         <v>72.23809523809524</v>
       </c>
-      <c r="D124">
-        <v>8</v>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E124">
         <v>1</v>
@@ -4723,8 +4969,10 @@
       <c r="C125">
         <v>54.87142857142857</v>
       </c>
-      <c r="D125">
-        <v>4</v>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E125">
         <v>0</v>
@@ -4758,8 +5006,10 @@
       <c r="C126">
         <v>67.32978723404256</v>
       </c>
-      <c r="D126">
-        <v>6</v>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E126">
         <v>1</v>
@@ -4793,8 +5043,10 @@
       <c r="C127">
         <v>61.09302325581395</v>
       </c>
-      <c r="D127">
-        <v>6</v>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E127">
         <v>1</v>
@@ -4828,8 +5080,10 @@
       <c r="C128">
         <v>44.03409090909091</v>
       </c>
-      <c r="D128">
-        <v>4</v>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E128">
         <v>1</v>
@@ -4863,8 +5117,10 @@
       <c r="C129">
         <v>20.08139534883721</v>
       </c>
-      <c r="D129">
-        <v>1</v>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E129">
         <v>1</v>
@@ -4898,8 +5154,10 @@
       <c r="C130">
         <v>54.90217391304348</v>
       </c>
-      <c r="D130">
-        <v>4</v>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E130">
         <v>0</v>
@@ -4933,8 +5191,10 @@
       <c r="C131">
         <v>67.33333333333333</v>
       </c>
-      <c r="D131">
-        <v>7</v>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E131">
         <v>1</v>
@@ -4968,8 +5228,10 @@
       <c r="C132">
         <v>12.02380952380952</v>
       </c>
-      <c r="D132">
-        <v>1</v>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E132">
         <v>1</v>
@@ -5003,8 +5265,10 @@
       <c r="C133">
         <v>53.18055555555556</v>
       </c>
-      <c r="D133">
-        <v>4</v>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E133">
         <v>0</v>
@@ -5038,8 +5302,10 @@
       <c r="C134">
         <v>61.26086956521739</v>
       </c>
-      <c r="D134">
-        <v>6</v>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E134">
         <v>1</v>
@@ -5073,8 +5339,10 @@
       <c r="C135">
         <v>19.63095238095238</v>
       </c>
-      <c r="D135">
-        <v>1</v>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E135">
         <v>1</v>
@@ -5108,8 +5376,10 @@
       <c r="C136">
         <v>51.60294117647059</v>
       </c>
-      <c r="D136">
-        <v>3</v>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E136">
         <v>0</v>
@@ -5143,8 +5413,10 @@
       <c r="C137">
         <v>29.41489361702127</v>
       </c>
-      <c r="D137">
-        <v>2</v>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E137">
         <v>1</v>
@@ -5178,8 +5450,10 @@
       <c r="C138">
         <v>72.45555555555555</v>
       </c>
-      <c r="D138">
-        <v>8</v>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E138">
         <v>1</v>
@@ -5213,8 +5487,10 @@
       <c r="C139">
         <v>59.85185185185185</v>
       </c>
-      <c r="D139">
-        <v>5</v>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E139">
         <v>0</v>
@@ -5248,8 +5524,10 @@
       <c r="C140">
         <v>52.5945945945946</v>
       </c>
-      <c r="D140">
-        <v>4</v>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E140">
         <v>0</v>
@@ -5283,8 +5561,10 @@
       <c r="C141">
         <v>86.04651162790697</v>
       </c>
-      <c r="D141">
-        <v>10</v>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E141">
         <v>1</v>
@@ -5318,8 +5598,10 @@
       <c r="C142">
         <v>50.25555555555555</v>
       </c>
-      <c r="D142">
-        <v>4</v>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E142">
         <v>1</v>
@@ -5353,8 +5635,10 @@
       <c r="C143">
         <v>66.06666666666666</v>
       </c>
-      <c r="D143">
-        <v>6</v>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E143">
         <v>1</v>
@@ -5388,8 +5672,10 @@
       <c r="C144">
         <v>60.5625</v>
       </c>
-      <c r="D144">
-        <v>5</v>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E144">
         <v>1</v>
@@ -5423,8 +5709,10 @@
       <c r="C145">
         <v>71.04545454545455</v>
       </c>
-      <c r="D145">
-        <v>7</v>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E145">
         <v>1</v>
@@ -5458,8 +5746,10 @@
       <c r="C146">
         <v>53.05319148936171</v>
       </c>
-      <c r="D146">
-        <v>4</v>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E146">
         <v>0</v>
@@ -5493,8 +5783,10 @@
       <c r="C147">
         <v>51.39705882352941</v>
       </c>
-      <c r="D147">
-        <v>3</v>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E147">
         <v>0</v>
@@ -5528,8 +5820,10 @@
       <c r="C148">
         <v>20.81111111111111</v>
       </c>
-      <c r="D148">
-        <v>2</v>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E148">
         <v>1</v>
@@ -5563,8 +5857,10 @@
       <c r="C149">
         <v>67.92553191489361</v>
       </c>
-      <c r="D149">
-        <v>7</v>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E149">
         <v>1</v>
@@ -5598,8 +5894,10 @@
       <c r="C150">
         <v>80.47619047619048</v>
       </c>
-      <c r="D150">
-        <v>10</v>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E150">
         <v>1</v>
@@ -5633,8 +5931,10 @@
       <c r="C151">
         <v>32.05</v>
       </c>
-      <c r="D151">
-        <v>3</v>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E151">
         <v>1</v>
@@ -5668,8 +5968,10 @@
       <c r="C152">
         <v>51.65</v>
       </c>
-      <c r="D152">
-        <v>5</v>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E152">
         <v>1</v>
@@ -5703,8 +6005,10 @@
       <c r="C153">
         <v>79.55681818181819</v>
       </c>
-      <c r="D153">
-        <v>9</v>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E153">
         <v>1</v>
@@ -5738,8 +6042,10 @@
       <c r="C154">
         <v>43.4390243902439</v>
       </c>
-      <c r="D154">
-        <v>3</v>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E154">
         <v>1</v>
@@ -5773,8 +6079,10 @@
       <c r="C155">
         <v>76.3452380952381</v>
       </c>
-      <c r="D155">
-        <v>8</v>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E155">
         <v>1</v>
@@ -5808,8 +6116,10 @@
       <c r="C156">
         <v>44.45121951219512</v>
       </c>
-      <c r="D156">
-        <v>4</v>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E156">
         <v>1</v>
@@ -5843,8 +6153,10 @@
       <c r="C157">
         <v>76.70652173913044</v>
       </c>
-      <c r="D157">
-        <v>9</v>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E157">
         <v>1</v>
@@ -5878,8 +6190,10 @@
       <c r="C158">
         <v>68.28749999999999</v>
       </c>
-      <c r="D158">
-        <v>7</v>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E158">
         <v>1</v>
@@ -5913,8 +6227,10 @@
       <c r="C159">
         <v>18.86764705882353</v>
       </c>
-      <c r="D159">
-        <v>1</v>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E159">
         <v>1</v>
@@ -5948,8 +6264,10 @@
       <c r="C160">
         <v>77.0625</v>
       </c>
-      <c r="D160">
-        <v>9</v>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E160">
         <v>1</v>
@@ -5983,8 +6301,10 @@
       <c r="C161">
         <v>54.25</v>
       </c>
-      <c r="D161">
-        <v>4</v>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E161">
         <v>1</v>
@@ -6018,8 +6338,10 @@
       <c r="C162">
         <v>68.30645161290323</v>
       </c>
-      <c r="D162">
-        <v>7</v>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E162">
         <v>1</v>
@@ -6053,8 +6375,10 @@
       <c r="C163">
         <v>58.95</v>
       </c>
-      <c r="D163">
-        <v>5</v>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E163">
         <v>1</v>
@@ -6088,8 +6412,10 @@
       <c r="C164">
         <v>73.1547619047619</v>
       </c>
-      <c r="D164">
-        <v>8</v>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E164">
         <v>1</v>
@@ -6123,8 +6449,10 @@
       <c r="C165">
         <v>64.7948717948718</v>
       </c>
-      <c r="D165">
-        <v>6</v>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E165">
         <v>1</v>
@@ -6158,8 +6486,10 @@
       <c r="C166">
         <v>82.54054054054055</v>
       </c>
-      <c r="D166">
-        <v>10</v>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E166">
         <v>1</v>
@@ -6193,8 +6523,10 @@
       <c r="C167">
         <v>48.40000000000001</v>
       </c>
-      <c r="D167">
-        <v>3</v>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E167">
         <v>1</v>
@@ -6228,8 +6560,10 @@
       <c r="C168">
         <v>72.85526315789474</v>
       </c>
-      <c r="D168">
-        <v>8</v>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E168">
         <v>1</v>
@@ -6263,8 +6597,10 @@
       <c r="C169">
         <v>18.83333333333333</v>
       </c>
-      <c r="D169">
-        <v>1</v>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E169">
         <v>1</v>
@@ -6298,8 +6634,10 @@
       <c r="C170">
         <v>37.2741935483871</v>
       </c>
-      <c r="D170">
-        <v>2</v>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E170">
         <v>1</v>
@@ -6333,8 +6671,10 @@
       <c r="C171">
         <v>83.4375</v>
       </c>
-      <c r="D171">
-        <v>10</v>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E171">
         <v>1</v>
@@ -6368,8 +6708,10 @@
       <c r="C172">
         <v>38.85</v>
       </c>
-      <c r="D172">
-        <v>2</v>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E172">
         <v>1</v>
@@ -6403,8 +6745,10 @@
       <c r="C173">
         <v>77.44736842105263</v>
       </c>
-      <c r="D173">
-        <v>9</v>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E173">
         <v>1</v>
@@ -6438,8 +6782,10 @@
       <c r="C174">
         <v>58.86170212765958</v>
       </c>
-      <c r="D174">
-        <v>5</v>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E174">
         <v>1</v>
@@ -6473,8 +6819,10 @@
       <c r="C175">
         <v>53.55714285714285</v>
       </c>
-      <c r="D175">
-        <v>4</v>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E175">
         <v>1</v>
@@ -6508,8 +6856,10 @@
       <c r="C176">
         <v>48.30882352941177</v>
       </c>
-      <c r="D176">
-        <v>3</v>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E176">
         <v>1</v>
@@ -6543,8 +6893,10 @@
       <c r="C177">
         <v>64.46052631578948</v>
       </c>
-      <c r="D177">
-        <v>6</v>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E177">
         <v>1</v>
@@ -6578,8 +6930,10 @@
       <c r="C178">
         <v>77.09999999999999</v>
       </c>
-      <c r="D178">
-        <v>9</v>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E178">
         <v>1</v>
@@ -6613,8 +6967,10 @@
       <c r="C179">
         <v>68.42045454545455</v>
       </c>
-      <c r="D179">
-        <v>7</v>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E179">
         <v>1</v>
@@ -6648,8 +7004,10 @@
       <c r="C180">
         <v>54.01351351351352</v>
       </c>
-      <c r="D180">
-        <v>4</v>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E180">
         <v>1</v>
@@ -6683,8 +7041,10 @@
       <c r="C181">
         <v>77.14285714285714</v>
       </c>
-      <c r="D181">
-        <v>9</v>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E181">
         <v>1</v>
@@ -6718,8 +7078,10 @@
       <c r="C182">
         <v>47.56756756756756</v>
       </c>
-      <c r="D182">
-        <v>3</v>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E182">
         <v>1</v>
@@ -6753,8 +7115,10 @@
       <c r="C183">
         <v>17.89285714285714</v>
       </c>
-      <c r="D183">
-        <v>1</v>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E183">
         <v>1</v>
@@ -6788,8 +7152,10 @@
       <c r="C184">
         <v>64.78947368421052</v>
       </c>
-      <c r="D184">
-        <v>6</v>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E184">
         <v>1</v>
@@ -6823,8 +7189,10 @@
       <c r="C185">
         <v>72.96875</v>
       </c>
-      <c r="D185">
-        <v>8</v>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E185">
         <v>1</v>
@@ -6858,8 +7226,10 @@
       <c r="C186">
         <v>36.96153846153846</v>
       </c>
-      <c r="D186">
-        <v>2</v>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E186">
         <v>1</v>
@@ -6893,8 +7263,10 @@
       <c r="C187">
         <v>68.64285714285714</v>
       </c>
-      <c r="D187">
-        <v>7</v>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E187">
         <v>1</v>
@@ -6928,8 +7300,10 @@
       <c r="C188">
         <v>83.03030303030303</v>
       </c>
-      <c r="D188">
-        <v>10</v>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E188">
         <v>1</v>
@@ -6963,8 +7337,10 @@
       <c r="C189">
         <v>47.32432432432432</v>
       </c>
-      <c r="D189">
-        <v>3</v>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E189">
         <v>1</v>
@@ -6998,8 +7374,10 @@
       <c r="C190">
         <v>18.21428571428572</v>
       </c>
-      <c r="D190">
-        <v>1</v>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E190">
         <v>1</v>
@@ -7033,8 +7411,10 @@
       <c r="C191">
         <v>64.72368421052632</v>
       </c>
-      <c r="D191">
-        <v>6</v>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E191">
         <v>1</v>
@@ -7068,8 +7448,10 @@
       <c r="C192">
         <v>59.30434782608695</v>
       </c>
-      <c r="D192">
-        <v>5</v>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E192">
         <v>1</v>
@@ -7103,8 +7485,10 @@
       <c r="C193">
         <v>35.64634146341464</v>
       </c>
-      <c r="D193">
-        <v>2</v>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E193">
         <v>1</v>
@@ -7138,8 +7522,10 @@
       <c r="C194">
         <v>53.67948717948718</v>
       </c>
-      <c r="D194">
-        <v>4</v>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E194">
         <v>1</v>
@@ -7173,8 +7559,10 @@
       <c r="C195">
         <v>59.45</v>
       </c>
-      <c r="D195">
-        <v>5</v>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E195">
         <v>1</v>
@@ -7208,8 +7596,10 @@
       <c r="C196">
         <v>72.94285714285715</v>
       </c>
-      <c r="D196">
-        <v>8</v>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E196">
         <v>1</v>
@@ -7243,8 +7633,10 @@
       <c r="C197">
         <v>83.06060606060606</v>
       </c>
-      <c r="D197">
-        <v>10</v>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E197">
         <v>1</v>
@@ -7278,8 +7670,10 @@
       <c r="C198">
         <v>74.51388888888889</v>
       </c>
-      <c r="D198">
-        <v>9</v>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E198">
         <v>1</v>
@@ -7313,8 +7707,10 @@
       <c r="C199">
         <v>78.515625</v>
       </c>
-      <c r="D199">
-        <v>10</v>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E199">
         <v>1</v>
@@ -7348,8 +7744,10 @@
       <c r="C200">
         <v>78.46969696969697</v>
       </c>
-      <c r="D200">
-        <v>10</v>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E200">
         <v>1</v>
@@ -7383,8 +7781,10 @@
       <c r="C201">
         <v>56.3125</v>
       </c>
-      <c r="D201">
-        <v>4</v>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E201">
         <v>1</v>
@@ -7418,8 +7818,10 @@
       <c r="C202">
         <v>55.14705882352941</v>
       </c>
-      <c r="D202">
-        <v>4</v>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E202">
         <v>1</v>
@@ -7453,8 +7855,10 @@
       <c r="C203">
         <v>63.24242424242424</v>
       </c>
-      <c r="D203">
-        <v>6</v>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E203">
         <v>1</v>
@@ -7488,8 +7892,10 @@
       <c r="C204">
         <v>28.76388888888889</v>
       </c>
-      <c r="D204">
-        <v>1</v>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E204">
         <v>1</v>
@@ -7523,8 +7929,10 @@
       <c r="C205">
         <v>67.08571428571429</v>
       </c>
-      <c r="D205">
-        <v>7</v>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E205">
         <v>1</v>
@@ -7558,8 +7966,10 @@
       <c r="C206">
         <v>74.51612903225806</v>
       </c>
-      <c r="D206">
-        <v>9</v>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E206">
         <v>1</v>
@@ -7593,8 +8003,10 @@
       <c r="C207">
         <v>69.76470588235294</v>
       </c>
-      <c r="D207">
-        <v>8</v>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E207">
         <v>1</v>
@@ -7628,8 +8040,10 @@
       <c r="C208">
         <v>59.07352941176471</v>
       </c>
-      <c r="D208">
-        <v>5</v>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E208">
         <v>1</v>
@@ -7663,8 +8077,10 @@
       <c r="C209">
         <v>41.06451612903226</v>
       </c>
-      <c r="D209">
-        <v>2</v>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E209">
         <v>1</v>
@@ -7698,8 +8114,10 @@
       <c r="C210">
         <v>59.15151515151515</v>
       </c>
-      <c r="D210">
-        <v>5</v>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E210">
         <v>1</v>
@@ -7733,8 +8151,10 @@
       <c r="C211">
         <v>29.28048780487805</v>
       </c>
-      <c r="D211">
-        <v>1</v>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E211">
         <v>1</v>
@@ -7768,8 +8188,10 @@
       <c r="C212">
         <v>50.275</v>
       </c>
-      <c r="D212">
-        <v>3</v>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E212">
         <v>1</v>
@@ -7803,8 +8225,10 @@
       <c r="C213">
         <v>69.6875</v>
       </c>
-      <c r="D213">
-        <v>8</v>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E213">
         <v>1</v>
@@ -7838,8 +8262,10 @@
       <c r="C214">
         <v>49.66176470588235</v>
       </c>
-      <c r="D214">
-        <v>3</v>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E214">
         <v>1</v>
@@ -7873,8 +8299,10 @@
       <c r="C215">
         <v>67.61538461538461</v>
       </c>
-      <c r="D215">
-        <v>7</v>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E215">
         <v>1</v>
@@ -7908,8 +8336,10 @@
       <c r="C216">
         <v>42.22222222222222</v>
       </c>
-      <c r="D216">
-        <v>2</v>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E216">
         <v>1</v>
@@ -7943,8 +8373,10 @@
       <c r="C217">
         <v>64.04411764705883</v>
       </c>
-      <c r="D217">
-        <v>6</v>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E217">
         <v>1</v>
@@ -7978,8 +8410,10 @@
       <c r="C218">
         <v>50</v>
       </c>
-      <c r="D218">
-        <v>3</v>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E218">
         <v>1</v>
@@ -8013,8 +8447,10 @@
       <c r="C219">
         <v>73.765625</v>
       </c>
-      <c r="D219">
-        <v>9</v>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E219">
         <v>1</v>
@@ -8048,8 +8484,10 @@
       <c r="C220">
         <v>74.22058823529412</v>
       </c>
-      <c r="D220">
-        <v>9</v>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E220">
         <v>1</v>
@@ -8083,8 +8521,10 @@
       <c r="C221">
         <v>70.06756756756756</v>
       </c>
-      <c r="D221">
-        <v>8</v>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E221">
         <v>1</v>
@@ -8118,8 +8558,10 @@
       <c r="C222">
         <v>63.59090909090909</v>
       </c>
-      <c r="D222">
-        <v>6</v>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E222">
         <v>1</v>
@@ -8153,8 +8595,10 @@
       <c r="C223">
         <v>63.67948717948718</v>
       </c>
-      <c r="D223">
-        <v>6</v>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E223">
         <v>1</v>
@@ -8188,8 +8632,10 @@
       <c r="C224">
         <v>26.04054054054054</v>
       </c>
-      <c r="D224">
-        <v>1</v>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E224">
         <v>1</v>
@@ -8223,8 +8669,10 @@
       <c r="C225">
         <v>59.74285714285715</v>
       </c>
-      <c r="D225">
-        <v>5</v>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E225">
         <v>1</v>
@@ -8258,8 +8706,10 @@
       <c r="C226">
         <v>67.51785714285714</v>
       </c>
-      <c r="D226">
-        <v>7</v>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E226">
         <v>1</v>
@@ -8293,8 +8743,10 @@
       <c r="C227">
         <v>67.234375</v>
       </c>
-      <c r="D227">
-        <v>7</v>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E227">
         <v>1</v>
@@ -8328,8 +8780,10 @@
       <c r="C228">
         <v>42.01515151515152</v>
       </c>
-      <c r="D228">
-        <v>2</v>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E228">
         <v>1</v>
@@ -8363,8 +8817,10 @@
       <c r="C229">
         <v>55.73529411764706</v>
       </c>
-      <c r="D229">
-        <v>4</v>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E229">
         <v>1</v>
@@ -8398,8 +8854,10 @@
       <c r="C230">
         <v>49.72727272727273</v>
       </c>
-      <c r="D230">
-        <v>3</v>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E230">
         <v>1</v>
@@ -8433,8 +8891,10 @@
       <c r="C231">
         <v>59.38571428571429</v>
       </c>
-      <c r="D231">
-        <v>5</v>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E231">
         <v>1</v>
@@ -8468,8 +8928,10 @@
       <c r="C232">
         <v>69.98484848484848</v>
       </c>
-      <c r="D232">
-        <v>8</v>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E232">
         <v>1</v>
@@ -8503,8 +8965,10 @@
       <c r="C233">
         <v>41.37179487179487</v>
       </c>
-      <c r="D233">
-        <v>2</v>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E233">
         <v>1</v>
@@ -8538,8 +9002,10 @@
       <c r="C234">
         <v>26.32352941176471</v>
       </c>
-      <c r="D234">
-        <v>1</v>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E234">
         <v>1</v>
@@ -8573,8 +9039,10 @@
       <c r="C235">
         <v>78.86111111111111</v>
       </c>
-      <c r="D235">
-        <v>10</v>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E235">
         <v>1</v>
@@ -8608,8 +9076,10 @@
       <c r="C236">
         <v>55.17142857142858</v>
       </c>
-      <c r="D236">
-        <v>4</v>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E236">
         <v>1</v>
@@ -8643,8 +9113,10 @@
       <c r="C237">
         <v>78.57352941176471</v>
       </c>
-      <c r="D237">
-        <v>10</v>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E237">
         <v>1</v>
@@ -8678,8 +9150,10 @@
       <c r="C238">
         <v>73.98809523809524</v>
       </c>
-      <c r="D238">
-        <v>8</v>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E238">
         <v>1</v>
@@ -8713,8 +9187,10 @@
       <c r="C239">
         <v>17.51041666666667</v>
       </c>
-      <c r="D239">
-        <v>1</v>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E239">
         <v>1</v>
@@ -8748,8 +9224,10 @@
       <c r="C240">
         <v>78</v>
       </c>
-      <c r="D240">
-        <v>9</v>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E240">
         <v>1</v>
@@ -8783,8 +9261,10 @@
       <c r="C241">
         <v>55.69318181818181</v>
       </c>
-      <c r="D241">
-        <v>5</v>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E241">
         <v>1</v>
@@ -8818,8 +9298,10 @@
       <c r="C242">
         <v>68.96808510638297</v>
       </c>
-      <c r="D242">
-        <v>7</v>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E242">
         <v>1</v>
@@ -8853,8 +9335,10 @@
       <c r="C243">
         <v>39.79347826086956</v>
       </c>
-      <c r="D243">
-        <v>3</v>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E243">
         <v>1</v>
@@ -8888,8 +9372,10 @@
       <c r="C244">
         <v>68.7</v>
       </c>
-      <c r="D244">
-        <v>7</v>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E244">
         <v>1</v>
@@ -8923,8 +9409,10 @@
       <c r="C245">
         <v>54.80952380952381</v>
       </c>
-      <c r="D245">
-        <v>5</v>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E245">
         <v>1</v>
@@ -8958,8 +9446,10 @@
       <c r="C246">
         <v>62.95</v>
       </c>
-      <c r="D246">
-        <v>6</v>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E246">
         <v>1</v>
@@ -8993,8 +9483,10 @@
       <c r="C247">
         <v>77.65853658536585</v>
       </c>
-      <c r="D247">
-        <v>9</v>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E247">
         <v>1</v>
@@ -9028,8 +9520,10 @@
       <c r="C248">
         <v>48.12790697674419</v>
       </c>
-      <c r="D248">
-        <v>4</v>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E248">
         <v>1</v>
@@ -9063,8 +9557,10 @@
       <c r="C249">
         <v>15.19512195121951</v>
       </c>
-      <c r="D249">
-        <v>1</v>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E249">
         <v>1</v>
@@ -9098,8 +9594,10 @@
       <c r="C250">
         <v>25.34883720930232</v>
       </c>
-      <c r="D250">
-        <v>2</v>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E250">
         <v>1</v>
@@ -9133,8 +9631,10 @@
       <c r="C251">
         <v>47.94047619047619</v>
       </c>
-      <c r="D251">
-        <v>4</v>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E251">
         <v>1</v>
@@ -9168,8 +9668,10 @@
       <c r="C252">
         <v>82.65116279069767</v>
       </c>
-      <c r="D252">
-        <v>10</v>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E252">
         <v>1</v>
@@ -9203,8 +9705,10 @@
       <c r="C253">
         <v>62.86363636363636</v>
       </c>
-      <c r="D253">
-        <v>6</v>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E253">
         <v>1</v>
@@ -9238,8 +9742,10 @@
       <c r="C254">
         <v>82.66666666666666</v>
       </c>
-      <c r="D254">
-        <v>10</v>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E254">
         <v>1</v>
@@ -9273,8 +9779,10 @@
       <c r="C255">
         <v>26.45555555555556</v>
       </c>
-      <c r="D255">
-        <v>2</v>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E255">
         <v>1</v>
@@ -9308,8 +9816,10 @@
       <c r="C256">
         <v>38.73913043478261</v>
       </c>
-      <c r="D256">
-        <v>3</v>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E256">
         <v>1</v>
@@ -9343,8 +9853,10 @@
       <c r="C257">
         <v>74.12790697674419</v>
       </c>
-      <c r="D257">
-        <v>8</v>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E257">
         <v>1</v>
@@ -9378,8 +9890,10 @@
       <c r="C258">
         <v>68.53571428571428</v>
       </c>
-      <c r="D258">
-        <v>7</v>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E258">
         <v>1</v>
@@ -9413,8 +9927,10 @@
       <c r="C259">
         <v>82.3953488372093</v>
       </c>
-      <c r="D259">
-        <v>10</v>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E259">
         <v>1</v>
@@ -9448,8 +9964,10 @@
       <c r="C260">
         <v>73.51086956521739</v>
       </c>
-      <c r="D260">
-        <v>8</v>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E260">
         <v>1</v>
@@ -9483,8 +10001,10 @@
       <c r="C261">
         <v>48.48837209302326</v>
       </c>
-      <c r="D261">
-        <v>4</v>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E261">
         <v>1</v>
@@ -9518,8 +10038,10 @@
       <c r="C262">
         <v>77.47777777777779</v>
       </c>
-      <c r="D262">
-        <v>9</v>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E262">
         <v>1</v>
@@ -9553,8 +10075,10 @@
       <c r="C263">
         <v>62.25555555555556</v>
       </c>
-      <c r="D263">
-        <v>6</v>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E263">
         <v>1</v>
@@ -9588,8 +10112,10 @@
       <c r="C264">
         <v>62.70454545454545</v>
       </c>
-      <c r="D264">
-        <v>6</v>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E264">
         <v>1</v>
@@ -9623,8 +10149,10 @@
       <c r="C265">
         <v>14.53191489361702</v>
       </c>
-      <c r="D265">
-        <v>1</v>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E265">
         <v>1</v>
@@ -9658,8 +10186,10 @@
       <c r="C266">
         <v>68.64772727272728</v>
       </c>
-      <c r="D266">
-        <v>7</v>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="E266">
         <v>1</v>
@@ -9693,8 +10223,10 @@
       <c r="C267">
         <v>39.96739130434783</v>
       </c>
-      <c r="D267">
-        <v>3</v>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E267">
         <v>1</v>
@@ -9728,8 +10260,10 @@
       <c r="C268">
         <v>73.22222222222223</v>
       </c>
-      <c r="D268">
-        <v>8</v>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E268">
         <v>1</v>
@@ -9763,8 +10297,10 @@
       <c r="C269">
         <v>26.9468085106383</v>
       </c>
-      <c r="D269">
-        <v>2</v>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E269">
         <v>1</v>
@@ -9798,8 +10334,10 @@
       <c r="C270">
         <v>58</v>
       </c>
-      <c r="D270">
-        <v>5</v>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E270">
         <v>1</v>
@@ -9833,8 +10371,10 @@
       <c r="C271">
         <v>77.13953488372093</v>
       </c>
-      <c r="D271">
-        <v>9</v>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="E271">
         <v>1</v>
@@ -9868,8 +10408,10 @@
       <c r="C272">
         <v>47.32558139534883</v>
       </c>
-      <c r="D272">
-        <v>4</v>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="E272">
         <v>1</v>
@@ -9903,8 +10445,10 @@
       <c r="C273">
         <v>58.17391304347827</v>
       </c>
-      <c r="D273">
-        <v>5</v>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="E273">
         <v>1</v>
@@ -9938,8 +10482,10 @@
       <c r="C274">
         <v>14.87209302325581</v>
       </c>
-      <c r="D274">
-        <v>1</v>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E274">
         <v>1</v>
@@ -9973,8 +10519,10 @@
       <c r="C275">
         <v>83.27906976744185</v>
       </c>
-      <c r="D275">
-        <v>10</v>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E275">
         <v>1</v>
@@ -10008,8 +10556,10 @@
       <c r="C276">
         <v>40.44594594594595</v>
       </c>
-      <c r="D276">
-        <v>3</v>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="E276">
         <v>1</v>
@@ -10043,8 +10593,10 @@
       <c r="C277">
         <v>27.38636363636364</v>
       </c>
-      <c r="D277">
-        <v>2</v>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E277">
         <v>1</v>

</xml_diff>